<commit_message>
Added a new spreadsheet which compares BSBM v3 results showing the effect of the new Fast Join optimization
</commit_message>
<xml_diff>
--- a/Benchmarks/dotNetRDF BSBM v2 Benchmark.xlsx
+++ b/Benchmarks/dotNetRDF BSBM v2 Benchmark.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="19095" windowHeight="11985"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="65">
   <si>
     <t>BSBM Benchmarks</t>
   </si>
@@ -212,12 +212,15 @@
   <si>
     <t>Leviathan Engine - Version 0.5.1 (With experimental join speed boost optimisation) using Default Optimiser</t>
   </si>
+  <si>
+    <t>BSBM Benchmarks (v2)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +505,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -509,15 +515,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -577,6 +574,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -589,12 +592,27 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -612,11 +630,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="0"/>
@@ -703,6 +724,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
@@ -787,6 +809,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -859,6 +882,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -937,6 +961,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1006,6 +1031,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1084,6 +1110,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
@@ -1171,31 +1198,45 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="77498624"/>
-        <c:axId val="77504512"/>
+        <c:smooth val="0"/>
+        <c:axId val="104977920"/>
+        <c:axId val="104979456"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77498624"/>
+        <c:axId val="104977920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77504512"/>
+        <c:crossAx val="104979456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77504512"/>
+        <c:axId val="104979456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1214,19 +1255,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77498624"/>
+        <c:crossAx val="104977920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1238,7 +1284,17 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1256,11 +1312,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1311,6 +1370,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1362,6 +1422,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1413,6 +1474,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1464,6 +1526,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -1515,6 +1578,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1566,31 +1630,45 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="77029760"/>
-        <c:axId val="77031296"/>
+        <c:smooth val="0"/>
+        <c:axId val="104693120"/>
+        <c:axId val="104694912"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77029760"/>
+        <c:axId val="104693120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77031296"/>
+        <c:crossAx val="104694912"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77031296"/>
+        <c:axId val="104694912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1609,19 +1687,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77029760"/>
+        <c:crossAx val="104693120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1633,7 +1716,17 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1651,11 +1744,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1742,6 +1838,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1829,30 +1926,45 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="77732480"/>
-        <c:axId val="77734272"/>
+        <c:smooth val="0"/>
+        <c:axId val="104724736"/>
+        <c:axId val="105385984"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77732480"/>
+        <c:axId val="104724736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77734272"/>
+        <c:crossAx val="105385984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77734272"/>
+        <c:axId val="105385984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1871,18 +1983,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77732480"/>
+        <c:crossAx val="104724736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1894,7 +2012,17 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-GB"/>
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1912,11 +2040,14 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:overlay val="0"/>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1994,6 +2125,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -2081,6 +2213,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -2153,6 +2286,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -2216,30 +2350,45 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="78068736"/>
-        <c:axId val="78095104"/>
+        <c:smooth val="0"/>
+        <c:axId val="105460480"/>
+        <c:axId val="105462016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="78068736"/>
+        <c:axId val="105460480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78095104"/>
+        <c:crossAx val="105462016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78095104"/>
+        <c:axId val="105462016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -2258,18 +2407,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="78068736"/>
+        <c:crossAx val="105460480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -2484,6 +2639,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2518,6 +2674,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2693,15 +2850,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L166"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G163" sqref="G163"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -2716,37 +2873,37 @@
     <col min="12" max="12" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-    </row>
-    <row r="2" spans="1:12" ht="12.75" customHeight="1">
+    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+    </row>
+    <row r="2" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34" t="s">
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="54"/>
+      <c r="G3" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="H3" s="54"/>
+      <c r="I3" s="54"/>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -2784,23 +2941,23 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
-      <c r="K5" s="31"/>
-      <c r="L5" s="32"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="32"/>
+      <c r="I5" s="32"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>10</v>
       </c>
@@ -2838,7 +2995,7 @@
         <v>0.67859999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>50</v>
       </c>
@@ -2876,23 +3033,23 @@
         <v>9.2114499999999992</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
-      <c r="J8" s="31"/>
-      <c r="K8" s="31"/>
-      <c r="L8" s="32"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="B8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
+      <c r="G8" s="32"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>10</v>
       </c>
@@ -2930,7 +3087,7 @@
         <v>0.15872</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>50</v>
       </c>
@@ -2968,7 +3125,7 @@
         <v>1.4269400000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>100</v>
       </c>
@@ -3006,7 +3163,7 @@
         <v>2.36009</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>250</v>
       </c>
@@ -3044,23 +3201,23 @@
         <v>10.8939</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
-      <c r="A13" s="30" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="31"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31"/>
-      <c r="K13" s="31"/>
-      <c r="L13" s="32"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="B13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="32"/>
+      <c r="I13" s="32"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="33"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>10</v>
       </c>
@@ -3098,7 +3255,7 @@
         <v>0.10006</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>50</v>
       </c>
@@ -3136,7 +3293,7 @@
         <v>0.47710000000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>100</v>
       </c>
@@ -3174,7 +3331,7 @@
         <v>0.60307999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>250</v>
       </c>
@@ -3212,7 +3369,7 @@
         <v>2.4279500000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>500</v>
       </c>
@@ -3250,7 +3407,7 @@
         <v>6.1241000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>1000</v>
       </c>
@@ -3288,23 +3445,23 @@
         <v>20.924060000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:12">
-      <c r="A20" s="30" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="31"/>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31"/>
-      <c r="H20" s="31"/>
-      <c r="I20" s="31"/>
-      <c r="J20" s="31"/>
-      <c r="K20" s="31"/>
-      <c r="L20" s="32"/>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="32"/>
+      <c r="I20" s="32"/>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="33"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>10</v>
       </c>
@@ -3342,7 +3499,7 @@
         <v>9.5159999999999995E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>50</v>
       </c>
@@ -3380,7 +3537,7 @@
         <v>0.48758000000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>100</v>
       </c>
@@ -3418,23 +3575,23 @@
         <v>0.62190000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:12">
-      <c r="A24" s="30" t="s">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="31"/>
-      <c r="F24" s="31"/>
-      <c r="G24" s="31"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="31"/>
-      <c r="J24" s="31"/>
-      <c r="K24" s="31"/>
-      <c r="L24" s="32"/>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="33"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>10</v>
       </c>
@@ -3472,7 +3629,7 @@
         <v>5.9520000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>50</v>
       </c>
@@ -3510,7 +3667,7 @@
         <v>8.1089999999999995E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>100</v>
       </c>
@@ -3548,7 +3705,7 @@
         <v>0.11791</v>
       </c>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>250</v>
       </c>
@@ -3586,7 +3743,7 @@
         <v>0.46982000000000002</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>500</v>
       </c>
@@ -3624,7 +3781,7 @@
         <v>2.6088499999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>1000</v>
       </c>
@@ -3662,23 +3819,23 @@
         <v>22.22946</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="32"/>
-    </row>
-    <row r="32" spans="1:12">
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="32"/>
+      <c r="J31" s="32"/>
+      <c r="K31" s="32"/>
+      <c r="L31" s="33"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>10</v>
       </c>
@@ -3716,7 +3873,7 @@
         <v>5.713E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>50</v>
       </c>
@@ -3754,7 +3911,7 @@
         <v>7.9829999999999998E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>100</v>
       </c>
@@ -3792,7 +3949,7 @@
         <v>0.15442</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>250</v>
       </c>
@@ -3830,23 +3987,23 @@
         <v>0.75348999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
-      <c r="A36" s="30" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="31" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="32"/>
-    </row>
-    <row r="37" spans="1:12">
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
+      <c r="H36" s="32"/>
+      <c r="I36" s="32"/>
+      <c r="J36" s="32"/>
+      <c r="K36" s="32"/>
+      <c r="L36" s="33"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>10</v>
       </c>
@@ -3884,7 +4041,7 @@
         <v>5.7119999999999997E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>50</v>
       </c>
@@ -3922,7 +4079,7 @@
         <v>5.9990000000000002E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>100</v>
       </c>
@@ -3960,7 +4117,7 @@
         <v>7.3039999999999994E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>250</v>
       </c>
@@ -3998,7 +4155,7 @@
         <v>0.11734</v>
       </c>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>500</v>
       </c>
@@ -4036,7 +4193,7 @@
         <v>0.29250999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>1000</v>
       </c>
@@ -4074,7 +4231,7 @@
         <v>0.97650000000000003</v>
       </c>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>1500</v>
       </c>
@@ -4112,7 +4269,7 @@
         <v>2.5354999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>2000</v>
       </c>
@@ -4150,23 +4307,23 @@
         <v>4.3053800000000004</v>
       </c>
     </row>
-    <row r="45" spans="1:12">
-      <c r="A45" s="35" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="B45" s="35"/>
-      <c r="C45" s="35"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="35"/>
-      <c r="G45" s="35"/>
-      <c r="H45" s="35"/>
-      <c r="I45" s="35"/>
-      <c r="J45" s="35"/>
-      <c r="K45" s="35"/>
-      <c r="L45" s="35"/>
-    </row>
-    <row r="46" spans="1:12">
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="30"/>
+      <c r="J45" s="30"/>
+      <c r="K45" s="30"/>
+      <c r="L45" s="30"/>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>10</v>
       </c>
@@ -4204,7 +4361,7 @@
         <v>5.6520000000000001E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>50</v>
       </c>
@@ -4242,7 +4399,7 @@
         <v>6.3210000000000002E-2</v>
       </c>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>100</v>
       </c>
@@ -4280,7 +4437,7 @@
         <v>7.392E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>250</v>
       </c>
@@ -4318,7 +4475,7 @@
         <v>0.12199</v>
       </c>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>500</v>
       </c>
@@ -4356,7 +4513,7 @@
         <v>0.28231000000000001</v>
       </c>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>1000</v>
       </c>
@@ -4394,7 +4551,7 @@
         <v>0.97097999999999995</v>
       </c>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
         <v>1500</v>
       </c>
@@ -4432,7 +4589,7 @@
         <v>2.5520900000000002</v>
       </c>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
         <v>2000</v>
       </c>
@@ -4470,7 +4627,7 @@
         <v>4.2667900000000003</v>
       </c>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
         <v>2500</v>
       </c>
@@ -4508,7 +4665,7 @@
         <v>8.0111799999999995</v>
       </c>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
         <v>2785</v>
       </c>
@@ -4534,23 +4691,23 @@
       <c r="K55" s="8"/>
       <c r="L55" s="8"/>
     </row>
-    <row r="56" spans="1:12">
-      <c r="A56" s="54" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="52" t="s">
         <v>39</v>
       </c>
-      <c r="B56" s="54"/>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54"/>
-      <c r="E56" s="54"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="54"/>
-      <c r="H56" s="54"/>
-      <c r="I56" s="54"/>
-      <c r="J56" s="54"/>
-      <c r="K56" s="54"/>
-      <c r="L56" s="54"/>
-    </row>
-    <row r="57" spans="1:12">
+      <c r="B56" s="52"/>
+      <c r="C56" s="52"/>
+      <c r="D56" s="52"/>
+      <c r="E56" s="52"/>
+      <c r="F56" s="52"/>
+      <c r="G56" s="52"/>
+      <c r="H56" s="52"/>
+      <c r="I56" s="52"/>
+      <c r="J56" s="52"/>
+      <c r="K56" s="52"/>
+      <c r="L56" s="52"/>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="19">
         <v>10</v>
       </c>
@@ -4569,16 +4726,16 @@
       <c r="F57" s="19">
         <v>50</v>
       </c>
-      <c r="G57" s="37" t="s">
+      <c r="G57" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="H57" s="46"/>
-      <c r="I57" s="46"/>
-      <c r="J57" s="46"/>
-      <c r="K57" s="46"/>
-      <c r="L57" s="47"/>
-    </row>
-    <row r="58" spans="1:12">
+      <c r="H57" s="44"/>
+      <c r="I57" s="44"/>
+      <c r="J57" s="44"/>
+      <c r="K57" s="44"/>
+      <c r="L57" s="45"/>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="19">
         <v>50</v>
       </c>
@@ -4597,14 +4754,14 @@
       <c r="F58" s="19">
         <v>50</v>
       </c>
-      <c r="G58" s="48"/>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="49"/>
-      <c r="K58" s="49"/>
-      <c r="L58" s="50"/>
-    </row>
-    <row r="59" spans="1:12">
+      <c r="G58" s="46"/>
+      <c r="H58" s="47"/>
+      <c r="I58" s="47"/>
+      <c r="J58" s="47"/>
+      <c r="K58" s="47"/>
+      <c r="L58" s="48"/>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="19">
         <v>100</v>
       </c>
@@ -4623,14 +4780,14 @@
       <c r="F59" s="19">
         <v>50</v>
       </c>
-      <c r="G59" s="48"/>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="49"/>
-      <c r="K59" s="49"/>
-      <c r="L59" s="50"/>
-    </row>
-    <row r="60" spans="1:12">
+      <c r="G59" s="46"/>
+      <c r="H59" s="47"/>
+      <c r="I59" s="47"/>
+      <c r="J59" s="47"/>
+      <c r="K59" s="47"/>
+      <c r="L59" s="48"/>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="19">
         <v>250</v>
       </c>
@@ -4649,14 +4806,14 @@
       <c r="F60" s="19">
         <v>50</v>
       </c>
-      <c r="G60" s="48"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="49"/>
-      <c r="J60" s="49"/>
-      <c r="K60" s="49"/>
-      <c r="L60" s="50"/>
-    </row>
-    <row r="61" spans="1:12">
+      <c r="G60" s="46"/>
+      <c r="H60" s="47"/>
+      <c r="I60" s="47"/>
+      <c r="J60" s="47"/>
+      <c r="K60" s="47"/>
+      <c r="L60" s="48"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="19">
         <v>500</v>
       </c>
@@ -4675,14 +4832,14 @@
       <c r="F61" s="19">
         <v>50</v>
       </c>
-      <c r="G61" s="48"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="49"/>
-      <c r="J61" s="49"/>
-      <c r="K61" s="49"/>
-      <c r="L61" s="50"/>
-    </row>
-    <row r="62" spans="1:12">
+      <c r="G61" s="46"/>
+      <c r="H61" s="47"/>
+      <c r="I61" s="47"/>
+      <c r="J61" s="47"/>
+      <c r="K61" s="47"/>
+      <c r="L61" s="48"/>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="19">
         <v>1000</v>
       </c>
@@ -4701,14 +4858,14 @@
       <c r="F62" s="19">
         <v>50</v>
       </c>
-      <c r="G62" s="48"/>
-      <c r="H62" s="49"/>
-      <c r="I62" s="49"/>
-      <c r="J62" s="49"/>
-      <c r="K62" s="49"/>
-      <c r="L62" s="50"/>
-    </row>
-    <row r="63" spans="1:12">
+      <c r="G62" s="46"/>
+      <c r="H62" s="47"/>
+      <c r="I62" s="47"/>
+      <c r="J62" s="47"/>
+      <c r="K62" s="47"/>
+      <c r="L62" s="48"/>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="22">
         <v>1500</v>
       </c>
@@ -4727,14 +4884,14 @@
       <c r="F63" s="19">
         <v>50</v>
       </c>
-      <c r="G63" s="48"/>
-      <c r="H63" s="49"/>
-      <c r="I63" s="49"/>
-      <c r="J63" s="49"/>
-      <c r="K63" s="49"/>
-      <c r="L63" s="50"/>
-    </row>
-    <row r="64" spans="1:12">
+      <c r="G63" s="46"/>
+      <c r="H63" s="47"/>
+      <c r="I63" s="47"/>
+      <c r="J63" s="47"/>
+      <c r="K63" s="47"/>
+      <c r="L63" s="48"/>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="22">
         <v>2000</v>
       </c>
@@ -4753,14 +4910,14 @@
       <c r="F64" s="19">
         <v>50</v>
       </c>
-      <c r="G64" s="51"/>
-      <c r="H64" s="52"/>
-      <c r="I64" s="52"/>
-      <c r="J64" s="52"/>
-      <c r="K64" s="52"/>
-      <c r="L64" s="53"/>
-    </row>
-    <row r="65" spans="1:12">
+      <c r="G64" s="49"/>
+      <c r="H64" s="50"/>
+      <c r="I64" s="50"/>
+      <c r="J64" s="50"/>
+      <c r="K64" s="50"/>
+      <c r="L64" s="51"/>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="22">
         <v>2500</v>
       </c>
@@ -4798,23 +4955,23 @@
         <v>4.5999699999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="35" t="s">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="B66" s="35"/>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
-      <c r="F66" s="35"/>
-      <c r="G66" s="35"/>
-      <c r="H66" s="35"/>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
-    </row>
-    <row r="67" spans="1:12">
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="30"/>
+      <c r="J66" s="30"/>
+      <c r="K66" s="30"/>
+      <c r="L66" s="30"/>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>10</v>
       </c>
@@ -4852,7 +5009,7 @@
         <v>5.5449999999999999E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>50</v>
       </c>
@@ -4890,7 +5047,7 @@
         <v>6.019E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>100</v>
       </c>
@@ -4928,7 +5085,7 @@
         <v>0.70699999999999996</v>
       </c>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>250</v>
       </c>
@@ -4966,7 +5123,7 @@
         <v>0.10993</v>
       </c>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>500</v>
       </c>
@@ -5004,7 +5161,7 @@
         <v>0.25968999999999998</v>
       </c>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>1000</v>
       </c>
@@ -5042,7 +5199,7 @@
         <v>0.83623000000000003</v>
       </c>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
         <v>1500</v>
       </c>
@@ -5080,7 +5237,7 @@
         <v>1.5902000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
         <v>2000</v>
       </c>
@@ -5118,7 +5275,7 @@
         <v>2.8646699999999998</v>
       </c>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
         <v>2500</v>
       </c>
@@ -5156,39 +5313,39 @@
         <v>4.5697999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:12" ht="30" customHeight="1">
-      <c r="A76" s="36" t="s">
+    <row r="76" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="B76" s="36"/>
-      <c r="C76" s="36"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="36"/>
-      <c r="G76" s="36"/>
-      <c r="H76" s="36"/>
-      <c r="I76" s="36"/>
-      <c r="J76" s="36"/>
-      <c r="K76" s="36"/>
-      <c r="L76" s="36"/>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="A77" s="35" t="s">
+      <c r="B76" s="34"/>
+      <c r="C76" s="34"/>
+      <c r="D76" s="34"/>
+      <c r="E76" s="34"/>
+      <c r="F76" s="34"/>
+      <c r="G76" s="34"/>
+      <c r="H76" s="34"/>
+      <c r="I76" s="34"/>
+      <c r="J76" s="34"/>
+      <c r="K76" s="34"/>
+      <c r="L76" s="34"/>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="30" t="s">
         <v>52</v>
       </c>
-      <c r="B77" s="35"/>
-      <c r="C77" s="35"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
-      <c r="F77" s="35"/>
-      <c r="G77" s="35"/>
-      <c r="H77" s="35"/>
-      <c r="I77" s="35"/>
-      <c r="J77" s="35"/>
-      <c r="K77" s="35"/>
-      <c r="L77" s="35"/>
-    </row>
-    <row r="78" spans="1:12">
+      <c r="B77" s="30"/>
+      <c r="C77" s="30"/>
+      <c r="D77" s="30"/>
+      <c r="E77" s="30"/>
+      <c r="F77" s="30"/>
+      <c r="G77" s="30"/>
+      <c r="H77" s="30"/>
+      <c r="I77" s="30"/>
+      <c r="J77" s="30"/>
+      <c r="K77" s="30"/>
+      <c r="L77" s="30"/>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>10</v>
       </c>
@@ -5226,7 +5383,7 @@
         <v>5.8749999999999997E-2</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>50</v>
       </c>
@@ -5264,7 +5421,7 @@
         <v>6.6750000000000004E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>100</v>
       </c>
@@ -5302,7 +5459,7 @@
         <v>8.4390000000000007E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>250</v>
       </c>
@@ -5340,7 +5497,7 @@
         <v>0.21539</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>500</v>
       </c>
@@ -5378,7 +5535,7 @@
         <v>0.69338</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>1000</v>
       </c>
@@ -5416,7 +5573,7 @@
         <v>2.70932</v>
       </c>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
         <v>1500</v>
       </c>
@@ -5454,7 +5611,7 @@
         <v>6.3721300000000003</v>
       </c>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
         <v>2000</v>
       </c>
@@ -5480,7 +5637,7 @@
       <c r="K85" s="8"/>
       <c r="L85" s="8"/>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
         <v>2500</v>
       </c>
@@ -5506,23 +5663,23 @@
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
     </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="35" t="s">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="30" t="s">
         <v>55</v>
       </c>
-      <c r="B87" s="35"/>
-      <c r="C87" s="35"/>
-      <c r="D87" s="35"/>
-      <c r="E87" s="35"/>
-      <c r="F87" s="35"/>
-      <c r="G87" s="35"/>
-      <c r="H87" s="35"/>
-      <c r="I87" s="35"/>
-      <c r="J87" s="35"/>
-      <c r="K87" s="35"/>
-      <c r="L87" s="35"/>
-    </row>
-    <row r="88" spans="1:12">
+      <c r="B87" s="30"/>
+      <c r="C87" s="30"/>
+      <c r="D87" s="30"/>
+      <c r="E87" s="30"/>
+      <c r="F87" s="30"/>
+      <c r="G87" s="30"/>
+      <c r="H87" s="30"/>
+      <c r="I87" s="30"/>
+      <c r="J87" s="30"/>
+      <c r="K87" s="30"/>
+      <c r="L87" s="30"/>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>10</v>
       </c>
@@ -5560,7 +5717,7 @@
         <v>0.86519999999999997</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>50</v>
       </c>
@@ -5598,7 +5755,7 @@
         <v>9.6369999999999997E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>100</v>
       </c>
@@ -5636,7 +5793,7 @@
         <v>0.13392999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>250</v>
       </c>
@@ -5674,7 +5831,7 @@
         <v>0.33007999999999998</v>
       </c>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>500</v>
       </c>
@@ -5712,7 +5869,7 @@
         <v>0.86368999999999996</v>
       </c>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>1000</v>
       </c>
@@ -5738,7 +5895,7 @@
       <c r="K93" s="8"/>
       <c r="L93" s="8"/>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
         <v>1500</v>
       </c>
@@ -5764,7 +5921,7 @@
       <c r="K94" s="8"/>
       <c r="L94" s="8"/>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
         <v>2000</v>
       </c>
@@ -5790,7 +5947,7 @@
       <c r="K95" s="8"/>
       <c r="L95" s="8"/>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
         <v>2500</v>
       </c>
@@ -5816,23 +5973,23 @@
       <c r="K96" s="8"/>
       <c r="L96" s="8"/>
     </row>
-    <row r="97" spans="1:12">
-      <c r="A97" s="35" t="s">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B97" s="35"/>
-      <c r="C97" s="35"/>
-      <c r="D97" s="35"/>
-      <c r="E97" s="35"/>
-      <c r="F97" s="35"/>
-      <c r="G97" s="35"/>
-      <c r="H97" s="35"/>
-      <c r="I97" s="35"/>
-      <c r="J97" s="35"/>
-      <c r="K97" s="35"/>
-      <c r="L97" s="35"/>
-    </row>
-    <row r="98" spans="1:12">
+      <c r="B97" s="30"/>
+      <c r="C97" s="30"/>
+      <c r="D97" s="30"/>
+      <c r="E97" s="30"/>
+      <c r="F97" s="30"/>
+      <c r="G97" s="30"/>
+      <c r="H97" s="30"/>
+      <c r="I97" s="30"/>
+      <c r="J97" s="30"/>
+      <c r="K97" s="30"/>
+      <c r="L97" s="30"/>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>10</v>
       </c>
@@ -5870,7 +6027,7 @@
         <v>5.8299999999999998E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:12">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>50</v>
       </c>
@@ -5908,7 +6065,7 @@
         <v>6.6129999999999994E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:12">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>100</v>
       </c>
@@ -5946,7 +6103,7 @@
         <v>9.6589999999999995E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:12">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>250</v>
       </c>
@@ -5984,7 +6141,7 @@
         <v>0.22684000000000001</v>
       </c>
     </row>
-    <row r="102" spans="1:12">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>500</v>
       </c>
@@ -6022,7 +6179,7 @@
         <v>0.68789</v>
       </c>
     </row>
-    <row r="103" spans="1:12">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>1000</v>
       </c>
@@ -6060,7 +6217,7 @@
         <v>2.6724100000000002</v>
       </c>
     </row>
-    <row r="104" spans="1:12">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104" s="5">
         <v>1500</v>
       </c>
@@ -6098,7 +6255,7 @@
         <v>6.19869</v>
       </c>
     </row>
-    <row r="105" spans="1:12">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105" s="5">
         <v>2000</v>
       </c>
@@ -6124,7 +6281,7 @@
       <c r="K105" s="8"/>
       <c r="L105" s="8"/>
     </row>
-    <row r="106" spans="1:12">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106" s="5">
         <v>2500</v>
       </c>
@@ -6150,23 +6307,23 @@
       <c r="K106" s="8"/>
       <c r="L106" s="8"/>
     </row>
-    <row r="107" spans="1:12">
-      <c r="A107" s="35" t="s">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="B107" s="35"/>
-      <c r="C107" s="35"/>
-      <c r="D107" s="35"/>
-      <c r="E107" s="35"/>
-      <c r="F107" s="35"/>
-      <c r="G107" s="35"/>
-      <c r="H107" s="35"/>
-      <c r="I107" s="35"/>
-      <c r="J107" s="35"/>
-      <c r="K107" s="35"/>
-      <c r="L107" s="35"/>
-    </row>
-    <row r="108" spans="1:12">
+      <c r="B107" s="30"/>
+      <c r="C107" s="30"/>
+      <c r="D107" s="30"/>
+      <c r="E107" s="30"/>
+      <c r="F107" s="30"/>
+      <c r="G107" s="30"/>
+      <c r="H107" s="30"/>
+      <c r="I107" s="30"/>
+      <c r="J107" s="30"/>
+      <c r="K107" s="30"/>
+      <c r="L107" s="30"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <v>10</v>
       </c>
@@ -6204,7 +6361,7 @@
         <v>9.9529999999999993E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:12">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>50</v>
       </c>
@@ -6242,7 +6399,7 @@
         <v>0.10312</v>
       </c>
     </row>
-    <row r="110" spans="1:12">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>100</v>
       </c>
@@ -6280,7 +6437,7 @@
         <v>0.14133999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:12">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>250</v>
       </c>
@@ -6318,7 +6475,7 @@
         <v>0.32865</v>
       </c>
     </row>
-    <row r="112" spans="1:12">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <v>500</v>
       </c>
@@ -6356,7 +6513,7 @@
         <v>0.84436</v>
       </c>
     </row>
-    <row r="113" spans="1:12">
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <v>1000</v>
       </c>
@@ -6382,7 +6539,7 @@
       <c r="K113" s="8"/>
       <c r="L113" s="8"/>
     </row>
-    <row r="114" spans="1:12">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="5">
         <v>1500</v>
       </c>
@@ -6408,7 +6565,7 @@
       <c r="K114" s="8"/>
       <c r="L114" s="8"/>
     </row>
-    <row r="115" spans="1:12">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="5">
         <v>2000</v>
       </c>
@@ -6434,7 +6591,7 @@
       <c r="K115" s="8"/>
       <c r="L115" s="8"/>
     </row>
-    <row r="116" spans="1:12">
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="5">
         <v>2500</v>
       </c>
@@ -6460,23 +6617,23 @@
       <c r="K116" s="8"/>
       <c r="L116" s="8"/>
     </row>
-    <row r="117" spans="1:12">
-      <c r="A117" s="35" t="s">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A117" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B117" s="35"/>
-      <c r="C117" s="35"/>
-      <c r="D117" s="35"/>
-      <c r="E117" s="35"/>
-      <c r="F117" s="35"/>
-      <c r="G117" s="35"/>
-      <c r="H117" s="35"/>
-      <c r="I117" s="35"/>
-      <c r="J117" s="35"/>
-      <c r="K117" s="35"/>
-      <c r="L117" s="35"/>
-    </row>
-    <row r="118" spans="1:12">
+      <c r="B117" s="30"/>
+      <c r="C117" s="30"/>
+      <c r="D117" s="30"/>
+      <c r="E117" s="30"/>
+      <c r="F117" s="30"/>
+      <c r="G117" s="30"/>
+      <c r="H117" s="30"/>
+      <c r="I117" s="30"/>
+      <c r="J117" s="30"/>
+      <c r="K117" s="30"/>
+      <c r="L117" s="30"/>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="8">
         <v>10</v>
       </c>
@@ -6514,7 +6671,7 @@
         <v>6.0639999999999999E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:12">
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
         <v>50</v>
       </c>
@@ -6552,7 +6709,7 @@
         <v>6.4519999999999994E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:12">
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="8">
         <v>100</v>
       </c>
@@ -6590,7 +6747,7 @@
         <v>8.2610000000000003E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:12">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>250</v>
       </c>
@@ -6628,7 +6785,7 @@
         <v>0.18583</v>
       </c>
     </row>
-    <row r="122" spans="1:12">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="8">
         <v>500</v>
       </c>
@@ -6666,7 +6823,7 @@
         <v>0.56186999999999998</v>
       </c>
     </row>
-    <row r="123" spans="1:12">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
         <v>1000</v>
       </c>
@@ -6704,7 +6861,7 @@
         <v>1.9471499999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:12">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="5">
         <v>1500</v>
       </c>
@@ -6742,7 +6899,7 @@
         <v>4.6351300000000002</v>
       </c>
     </row>
-    <row r="125" spans="1:12">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="5">
         <v>2000</v>
       </c>
@@ -6768,7 +6925,7 @@
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="1:12">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="5">
         <v>2500</v>
       </c>
@@ -6794,23 +6951,23 @@
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="1:12">
-      <c r="A127" s="35" t="s">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A127" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B127" s="35"/>
-      <c r="C127" s="35"/>
-      <c r="D127" s="35"/>
-      <c r="E127" s="35"/>
-      <c r="F127" s="35"/>
-      <c r="G127" s="35"/>
-      <c r="H127" s="35"/>
-      <c r="I127" s="35"/>
-      <c r="J127" s="35"/>
-      <c r="K127" s="35"/>
-      <c r="L127" s="35"/>
-    </row>
-    <row r="128" spans="1:12">
+      <c r="B127" s="30"/>
+      <c r="C127" s="30"/>
+      <c r="D127" s="30"/>
+      <c r="E127" s="30"/>
+      <c r="F127" s="30"/>
+      <c r="G127" s="30"/>
+      <c r="H127" s="30"/>
+      <c r="I127" s="30"/>
+      <c r="J127" s="30"/>
+      <c r="K127" s="30"/>
+      <c r="L127" s="30"/>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="19">
         <v>10</v>
       </c>
@@ -6829,16 +6986,16 @@
       <c r="F128" s="19">
         <v>50</v>
       </c>
-      <c r="G128" s="37" t="s">
+      <c r="G128" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="H128" s="38"/>
-      <c r="I128" s="38"/>
-      <c r="J128" s="38"/>
-      <c r="K128" s="38"/>
-      <c r="L128" s="39"/>
-    </row>
-    <row r="129" spans="1:12">
+      <c r="H128" s="36"/>
+      <c r="I128" s="36"/>
+      <c r="J128" s="36"/>
+      <c r="K128" s="36"/>
+      <c r="L128" s="37"/>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="19">
         <v>50</v>
       </c>
@@ -6857,14 +7014,14 @@
       <c r="F129" s="19">
         <v>50</v>
       </c>
-      <c r="G129" s="40"/>
-      <c r="H129" s="41"/>
-      <c r="I129" s="41"/>
-      <c r="J129" s="41"/>
-      <c r="K129" s="41"/>
-      <c r="L129" s="42"/>
-    </row>
-    <row r="130" spans="1:12">
+      <c r="G129" s="38"/>
+      <c r="H129" s="39"/>
+      <c r="I129" s="39"/>
+      <c r="J129" s="39"/>
+      <c r="K129" s="39"/>
+      <c r="L129" s="40"/>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130" s="19">
         <v>100</v>
       </c>
@@ -6883,14 +7040,14 @@
       <c r="F130" s="19">
         <v>50</v>
       </c>
-      <c r="G130" s="40"/>
-      <c r="H130" s="41"/>
-      <c r="I130" s="41"/>
-      <c r="J130" s="41"/>
-      <c r="K130" s="41"/>
-      <c r="L130" s="42"/>
-    </row>
-    <row r="131" spans="1:12">
+      <c r="G130" s="38"/>
+      <c r="H130" s="39"/>
+      <c r="I130" s="39"/>
+      <c r="J130" s="39"/>
+      <c r="K130" s="39"/>
+      <c r="L130" s="40"/>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131" s="19">
         <v>250</v>
       </c>
@@ -6909,14 +7066,14 @@
       <c r="F131" s="19">
         <v>50</v>
       </c>
-      <c r="G131" s="40"/>
-      <c r="H131" s="41"/>
-      <c r="I131" s="41"/>
-      <c r="J131" s="41"/>
-      <c r="K131" s="41"/>
-      <c r="L131" s="42"/>
-    </row>
-    <row r="132" spans="1:12">
+      <c r="G131" s="38"/>
+      <c r="H131" s="39"/>
+      <c r="I131" s="39"/>
+      <c r="J131" s="39"/>
+      <c r="K131" s="39"/>
+      <c r="L131" s="40"/>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132" s="19">
         <v>500</v>
       </c>
@@ -6935,14 +7092,14 @@
       <c r="F132" s="19">
         <v>50</v>
       </c>
-      <c r="G132" s="40"/>
-      <c r="H132" s="41"/>
-      <c r="I132" s="41"/>
-      <c r="J132" s="41"/>
-      <c r="K132" s="41"/>
-      <c r="L132" s="42"/>
-    </row>
-    <row r="133" spans="1:12">
+      <c r="G132" s="38"/>
+      <c r="H132" s="39"/>
+      <c r="I132" s="39"/>
+      <c r="J132" s="39"/>
+      <c r="K132" s="39"/>
+      <c r="L132" s="40"/>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133" s="19">
         <v>1000</v>
       </c>
@@ -6961,14 +7118,14 @@
       <c r="F133" s="19">
         <v>50</v>
       </c>
-      <c r="G133" s="40"/>
-      <c r="H133" s="41"/>
-      <c r="I133" s="41"/>
-      <c r="J133" s="41"/>
-      <c r="K133" s="41"/>
-      <c r="L133" s="42"/>
-    </row>
-    <row r="134" spans="1:12">
+      <c r="G133" s="38"/>
+      <c r="H133" s="39"/>
+      <c r="I133" s="39"/>
+      <c r="J133" s="39"/>
+      <c r="K133" s="39"/>
+      <c r="L133" s="40"/>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134" s="22">
         <v>1500</v>
       </c>
@@ -6987,14 +7144,14 @@
       <c r="F134" s="19">
         <v>50</v>
       </c>
-      <c r="G134" s="40"/>
-      <c r="H134" s="41"/>
-      <c r="I134" s="41"/>
-      <c r="J134" s="41"/>
-      <c r="K134" s="41"/>
-      <c r="L134" s="42"/>
-    </row>
-    <row r="135" spans="1:12">
+      <c r="G134" s="38"/>
+      <c r="H134" s="39"/>
+      <c r="I134" s="39"/>
+      <c r="J134" s="39"/>
+      <c r="K134" s="39"/>
+      <c r="L134" s="40"/>
+    </row>
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135" s="22">
         <v>2000</v>
       </c>
@@ -7013,14 +7170,14 @@
       <c r="F135" s="19">
         <v>50</v>
       </c>
-      <c r="G135" s="40"/>
-      <c r="H135" s="41"/>
-      <c r="I135" s="41"/>
-      <c r="J135" s="41"/>
-      <c r="K135" s="41"/>
-      <c r="L135" s="42"/>
-    </row>
-    <row r="136" spans="1:12">
+      <c r="G135" s="38"/>
+      <c r="H135" s="39"/>
+      <c r="I135" s="39"/>
+      <c r="J135" s="39"/>
+      <c r="K135" s="39"/>
+      <c r="L135" s="40"/>
+    </row>
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136" s="22">
         <v>2500</v>
       </c>
@@ -7039,30 +7196,30 @@
       <c r="F136" s="19">
         <v>50</v>
       </c>
-      <c r="G136" s="43"/>
-      <c r="H136" s="44"/>
-      <c r="I136" s="44"/>
-      <c r="J136" s="44"/>
-      <c r="K136" s="44"/>
-      <c r="L136" s="45"/>
-    </row>
-    <row r="137" spans="1:12">
-      <c r="A137" s="35" t="s">
+      <c r="G136" s="41"/>
+      <c r="H136" s="42"/>
+      <c r="I136" s="42"/>
+      <c r="J136" s="42"/>
+      <c r="K136" s="42"/>
+      <c r="L136" s="43"/>
+    </row>
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A137" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="B137" s="35"/>
-      <c r="C137" s="35"/>
-      <c r="D137" s="35"/>
-      <c r="E137" s="35"/>
-      <c r="F137" s="35"/>
-      <c r="G137" s="35"/>
-      <c r="H137" s="35"/>
-      <c r="I137" s="35"/>
-      <c r="J137" s="35"/>
-      <c r="K137" s="35"/>
-      <c r="L137" s="35"/>
-    </row>
-    <row r="138" spans="1:12">
+      <c r="B137" s="30"/>
+      <c r="C137" s="30"/>
+      <c r="D137" s="30"/>
+      <c r="E137" s="30"/>
+      <c r="F137" s="30"/>
+      <c r="G137" s="30"/>
+      <c r="H137" s="30"/>
+      <c r="I137" s="30"/>
+      <c r="J137" s="30"/>
+      <c r="K137" s="30"/>
+      <c r="L137" s="30"/>
+    </row>
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138" s="8">
         <v>10</v>
       </c>
@@ -7100,7 +7257,7 @@
         <v>6.114E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:12">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139" s="8">
         <v>50</v>
       </c>
@@ -7138,7 +7295,7 @@
         <v>6.6350000000000006E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:12">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140" s="8">
         <v>100</v>
       </c>
@@ -7176,7 +7333,7 @@
         <v>8.6169999999999997E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:12">
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141" s="8">
         <v>250</v>
       </c>
@@ -7214,7 +7371,7 @@
         <v>0.20794000000000001</v>
       </c>
     </row>
-    <row r="142" spans="1:12">
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142" s="8">
         <v>500</v>
       </c>
@@ -7252,7 +7409,7 @@
         <v>0.62724999999999997</v>
       </c>
     </row>
-    <row r="143" spans="1:12">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143" s="8">
         <v>1000</v>
       </c>
@@ -7290,7 +7447,7 @@
         <v>2.3531499999999999</v>
       </c>
     </row>
-    <row r="144" spans="1:12">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144" s="5">
         <v>1500</v>
       </c>
@@ -7316,7 +7473,7 @@
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
     </row>
-    <row r="145" spans="1:12">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="5">
         <v>2000</v>
       </c>
@@ -7342,7 +7499,7 @@
       <c r="K145" s="3"/>
       <c r="L145" s="3"/>
     </row>
-    <row r="146" spans="1:12">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="5">
         <v>2500</v>
       </c>
@@ -7368,23 +7525,23 @@
       <c r="K146" s="3"/>
       <c r="L146" s="3"/>
     </row>
-    <row r="147" spans="1:12">
-      <c r="A147" s="35" t="s">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A147" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="B147" s="35"/>
-      <c r="C147" s="35"/>
-      <c r="D147" s="35"/>
-      <c r="E147" s="35"/>
-      <c r="F147" s="35"/>
-      <c r="G147" s="35"/>
-      <c r="H147" s="35"/>
-      <c r="I147" s="35"/>
-      <c r="J147" s="35"/>
-      <c r="K147" s="35"/>
-      <c r="L147" s="35"/>
-    </row>
-    <row r="148" spans="1:12">
+      <c r="B147" s="30"/>
+      <c r="C147" s="30"/>
+      <c r="D147" s="30"/>
+      <c r="E147" s="30"/>
+      <c r="F147" s="30"/>
+      <c r="G147" s="30"/>
+      <c r="H147" s="30"/>
+      <c r="I147" s="30"/>
+      <c r="J147" s="30"/>
+      <c r="K147" s="30"/>
+      <c r="L147" s="30"/>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="8">
         <v>10</v>
       </c>
@@ -7422,7 +7579,7 @@
         <v>6.0400000000000002E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:12">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="8">
         <v>50</v>
       </c>
@@ -7460,7 +7617,7 @@
         <v>6.3299999999999995E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:12">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="8">
         <v>100</v>
       </c>
@@ -7498,7 +7655,7 @@
         <v>8.1989999999999993E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:12">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="8">
         <v>250</v>
       </c>
@@ -7536,7 +7693,7 @@
         <v>0.20244999999999999</v>
       </c>
     </row>
-    <row r="152" spans="1:12">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="8">
         <v>500</v>
       </c>
@@ -7574,7 +7731,7 @@
         <v>0.62250000000000005</v>
       </c>
     </row>
-    <row r="153" spans="1:12">
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="8">
         <v>1000</v>
       </c>
@@ -7612,7 +7769,7 @@
         <v>2.3825500000000002</v>
       </c>
     </row>
-    <row r="154" spans="1:12">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="5">
         <v>1500</v>
       </c>
@@ -7638,7 +7795,7 @@
       <c r="K154" s="3"/>
       <c r="L154" s="3"/>
     </row>
-    <row r="155" spans="1:12">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="5">
         <v>2000</v>
       </c>
@@ -7664,7 +7821,7 @@
       <c r="K155" s="3"/>
       <c r="L155" s="3"/>
     </row>
-    <row r="156" spans="1:12">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="5">
         <v>2500</v>
       </c>
@@ -7690,23 +7847,23 @@
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
     </row>
-    <row r="157" spans="1:12">
-      <c r="A157" s="35" t="s">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B157" s="35"/>
-      <c r="C157" s="35"/>
-      <c r="D157" s="35"/>
-      <c r="E157" s="35"/>
-      <c r="F157" s="35"/>
-      <c r="G157" s="35"/>
-      <c r="H157" s="35"/>
-      <c r="I157" s="35"/>
-      <c r="J157" s="35"/>
-      <c r="K157" s="35"/>
-      <c r="L157" s="35"/>
-    </row>
-    <row r="158" spans="1:12">
+      <c r="B157" s="30"/>
+      <c r="C157" s="30"/>
+      <c r="D157" s="30"/>
+      <c r="E157" s="30"/>
+      <c r="F157" s="30"/>
+      <c r="G157" s="30"/>
+      <c r="H157" s="30"/>
+      <c r="I157" s="30"/>
+      <c r="J157" s="30"/>
+      <c r="K157" s="30"/>
+      <c r="L157" s="30"/>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="8">
         <v>10</v>
       </c>
@@ -7744,7 +7901,7 @@
         <v>5.9520000000000003E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:12">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="8">
         <v>50</v>
       </c>
@@ -7782,7 +7939,7 @@
         <v>6.837E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:12">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="8">
         <v>100</v>
       </c>
@@ -7820,7 +7977,7 @@
         <v>8.881E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:12">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161" s="8">
         <v>250</v>
       </c>
@@ -7858,7 +8015,7 @@
         <v>0.23047999999999999</v>
       </c>
     </row>
-    <row r="162" spans="1:12">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162" s="8">
         <v>500</v>
       </c>
@@ -7896,7 +8053,7 @@
         <v>0.70959000000000005</v>
       </c>
     </row>
-    <row r="163" spans="1:12">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163" s="8">
         <v>1000</v>
       </c>
@@ -7922,7 +8079,7 @@
       <c r="K163" s="3"/>
       <c r="L163" s="3"/>
     </row>
-    <row r="164" spans="1:12">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164" s="5">
         <v>1500</v>
       </c>
@@ -7948,7 +8105,7 @@
       <c r="K164" s="3"/>
       <c r="L164" s="3"/>
     </row>
-    <row r="165" spans="1:12">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165" s="5">
         <v>2000</v>
       </c>
@@ -7974,7 +8131,7 @@
       <c r="K165" s="3"/>
       <c r="L165" s="3"/>
     </row>
-    <row r="166" spans="1:12">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166" s="5">
         <v>2500</v>
       </c>
@@ -8002,6 +8159,16 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A5:L5"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:L3"/>
     <mergeCell ref="A157:L157"/>
     <mergeCell ref="A147:L147"/>
     <mergeCell ref="A24:L24"/>
@@ -8018,16 +8185,6 @@
     <mergeCell ref="G57:L64"/>
     <mergeCell ref="A56:L56"/>
     <mergeCell ref="A45:L45"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A5:L5"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="D3:F3"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8035,14 +8192,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -8057,46 +8214,46 @@
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
       <c r="D1" s="24"/>
       <c r="E1" s="24"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="55" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="56"/>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -8140,25 +8297,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>10</v>
       </c>
@@ -8202,7 +8359,7 @@
         <v>7.3139999999999997E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>50</v>
       </c>
@@ -8246,7 +8403,7 @@
         <v>8.9130000000000001E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>100</v>
       </c>
@@ -8290,7 +8447,7 @@
         <v>0.1135</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>250</v>
       </c>
@@ -8334,7 +8491,7 @@
         <v>0.22333</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>500</v>
       </c>
@@ -8378,7 +8535,7 @@
         <v>0.45689999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>1000</v>
       </c>
@@ -8422,7 +8579,7 @@
         <v>1.2563200000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1500</v>
       </c>
@@ -8450,7 +8607,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2000</v>
       </c>
@@ -8478,7 +8635,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2500</v>
       </c>
@@ -8521,14 +8678,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -8543,46 +8700,46 @@
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="55" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="56"/>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -8626,25 +8783,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="35" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-    </row>
-    <row r="6" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>10</v>
       </c>
@@ -8688,7 +8845,7 @@
         <v>6.8290000000000003E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>50</v>
       </c>
@@ -8716,7 +8873,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>100</v>
       </c>
@@ -8744,7 +8901,7 @@
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>250</v>
       </c>
@@ -8772,7 +8929,7 @@
       <c r="M9" s="3"/>
       <c r="N9" s="3"/>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>500</v>
       </c>
@@ -8800,7 +8957,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>1000</v>
       </c>
@@ -8828,7 +8985,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1500</v>
       </c>
@@ -8856,7 +9013,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2000</v>
       </c>
@@ -8884,7 +9041,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2500</v>
       </c>
@@ -8926,14 +9083,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N24"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
@@ -8949,46 +9106,46 @@
     <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
       <c r="D1" s="25"/>
       <c r="E1" s="25"/>
     </row>
-    <row r="2" spans="1:14" ht="18.75">
+    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
     </row>
-    <row r="3" spans="1:14" ht="15.75">
-      <c r="A3" s="34" t="s">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="54" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
+      <c r="B3" s="54"/>
+      <c r="C3" s="54"/>
       <c r="D3" s="55" t="s">
         <v>44</v>
       </c>
       <c r="E3" s="56"/>
-      <c r="F3" s="34" t="s">
+      <c r="F3" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34" t="s">
+      <c r="G3" s="54"/>
+      <c r="H3" s="54"/>
+      <c r="I3" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+      <c r="L3" s="54"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="54"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
@@ -9032,25 +9189,25 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="35"/>
-      <c r="C5" s="35"/>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
-      <c r="G5" s="35"/>
-      <c r="H5" s="35"/>
-      <c r="I5" s="35"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="35"/>
-      <c r="L5" s="35"/>
-      <c r="M5" s="35"/>
-      <c r="N5" s="35"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="30"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="30"/>
+      <c r="K5" s="30"/>
+      <c r="L5" s="30"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="30"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>10</v>
       </c>
@@ -9094,7 +9251,7 @@
         <v>0.20480999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>50</v>
       </c>
@@ -9138,7 +9295,7 @@
         <v>0.13469999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>100</v>
       </c>
@@ -9182,7 +9339,7 @@
         <v>0.22617000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>250</v>
       </c>
@@ -9226,7 +9383,7 @@
         <v>0.39478000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>500</v>
       </c>
@@ -9254,7 +9411,7 @@
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>1000</v>
       </c>
@@ -9282,7 +9439,7 @@
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>1500</v>
       </c>
@@ -9310,7 +9467,7 @@
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>2000</v>
       </c>
@@ -9338,7 +9495,7 @@
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>2500</v>
       </c>
@@ -9366,25 +9523,25 @@
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="35" t="s">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="B15" s="35"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="35"/>
-      <c r="L15" s="35"/>
-      <c r="M15" s="35"/>
-      <c r="N15" s="35"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="30"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>10</v>
       </c>
@@ -9424,7 +9581,7 @@
         <v>0.11179</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>50</v>
       </c>
@@ -9464,7 +9621,7 @@
         <v>0.15948000000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>100</v>
       </c>
@@ -9504,7 +9661,7 @@
         <v>0.23547999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>250</v>
       </c>
@@ -9544,7 +9701,7 @@
         <v>0.56594</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>500</v>
       </c>
@@ -9584,7 +9741,7 @@
         <v>1.5053399999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>1000</v>
       </c>
@@ -9612,7 +9769,7 @@
       <c r="M21" s="3"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
         <v>1500</v>
       </c>
@@ -9640,7 +9797,7 @@
       <c r="M22" s="3"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>2000</v>
       </c>
@@ -9668,7 +9825,7 @@
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>2500</v>
       </c>
@@ -9712,19 +9869,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="5">
         <v>10</v>
@@ -9754,7 +9911,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
         <v>40</v>
       </c>
@@ -9786,7 +9943,7 @@
         <v>229.36500000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
         <v>38</v>
       </c>
@@ -9818,7 +9975,7 @@
         <v>522.19100000000003</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="16" t="s">
         <v>32</v>
       </c>
@@ -9848,7 +10005,7 @@
       </c>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>33</v>
       </c>
@@ -9870,7 +10027,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
         <v>36</v>
       </c>
@@ -9896,7 +10053,7 @@
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
         <v>34</v>
       </c>
@@ -9916,7 +10073,7 @@
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>35</v>
       </c>
@@ -9942,7 +10099,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
     </row>
   </sheetData>
@@ -9952,19 +10109,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3"/>
       <c r="B1" s="3">
         <v>10</v>
@@ -9994,7 +10151,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>51</v>
       </c>
@@ -10010,7 +10167,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>49</v>
       </c>
@@ -10032,7 +10189,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>47</v>
       </c>
@@ -10058,7 +10215,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
         <v>40</v>
       </c>
@@ -10091,13 +10248,13 @@
       </c>
       <c r="N5" s="27"/>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N6" s="27"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N7" s="27"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N8" s="27"/>
     </row>
   </sheetData>

</xml_diff>